<commit_message>
resolvido problema de usuarios da licença business premium, não listava
</commit_message>
<xml_diff>
--- a/LICENCIAMENTO MICROSOFT (1).xlsx
+++ b/LICENCIAMENTO MICROSOFT (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Braun\Documents\Licenciamento Microsoft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D23C6DE-AC9C-4F54-BEFD-AA22E33D51C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A11CFC-3AAF-45EB-9A73-9772E17298AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{026E40E1-97C9-4270-991D-E9C082A430FB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="658">
   <si>
     <t>setor</t>
   </si>
@@ -2043,7 +2043,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2055,12 +2055,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2152,7 +2154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2195,9 +2197,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2534,11 +2533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F403300F-DC30-4742-B09D-03B69867D524}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14:R182"/>
+      <selection activeCell="R163" sqref="R163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2551,8 +2549,8 @@
     <col min="6" max="8" width="36.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="76.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.109375" customWidth="1"/>
     <col min="15" max="15" width="14.109375" style="22" customWidth="1"/>
@@ -2622,7 +2620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2678,7 +2676,7 @@
       <c r="Q2" s="1">
         <v>1</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="25">
         <f>IF(N2&lt;=12,N2*P2,O2)</f>
         <v>1495.4166666666665</v>
       </c>
@@ -2686,7 +2684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2741,7 +2739,7 @@
       <c r="Q3" s="1">
         <v>1</v>
       </c>
-      <c r="R3" s="24">
+      <c r="R3" s="25">
         <f>IF(N3&lt;=12,N3*P3,O3)</f>
         <v>1663</v>
       </c>
@@ -2749,7 +2747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2805,7 +2803,7 @@
       <c r="Q4" s="1">
         <v>1</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="25">
         <f t="shared" ref="R4:R67" si="5">IF(N4&lt;=12,N4*P4,O4)</f>
         <v>298.8</v>
       </c>
@@ -2813,7 +2811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2868,7 +2866,7 @@
       <c r="Q5" s="1">
         <v>1</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2931,7 +2929,7 @@
       <c r="Q6" s="1">
         <v>1</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -2939,7 +2937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2994,7 +2992,7 @@
       <c r="Q7" s="1">
         <v>1</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3003,7 +3001,7 @@
       </c>
       <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -3058,7 +3056,7 @@
       <c r="Q8" s="1">
         <v>1</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3066,7 +3064,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3116,13 +3114,13 @@
         <v>1663</v>
       </c>
       <c r="P9" s="21">
-        <f t="shared" ref="P5:P13" si="8">O9/12</f>
+        <f t="shared" ref="P9:P13" si="8">O9/12</f>
         <v>138.58333333333334</v>
       </c>
       <c r="Q9" s="1">
         <v>1</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3130,7 +3128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3186,7 +3184,7 @@
       <c r="Q10" s="1">
         <v>1</v>
       </c>
-      <c r="R10" s="24">
+      <c r="R10" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3194,7 +3192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3250,7 +3248,7 @@
       <c r="Q11" s="1">
         <v>1</v>
       </c>
-      <c r="R11" s="24">
+      <c r="R11" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3258,7 +3256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -3314,7 +3312,7 @@
       <c r="Q12" s="1">
         <v>1</v>
       </c>
-      <c r="R12" s="24">
+      <c r="R12" s="25">
         <f t="shared" si="5"/>
         <v>1108.6666666666667</v>
       </c>
@@ -3322,7 +3320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3378,7 +3376,7 @@
       <c r="Q13" s="1">
         <v>1</v>
       </c>
-      <c r="R13" s="24">
+      <c r="R13" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3450,7 +3448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3506,7 +3504,7 @@
       <c r="Q15" s="1">
         <v>1</v>
       </c>
-      <c r="R15" s="24">
+      <c r="R15" s="25">
         <f t="shared" si="5"/>
         <v>1524.4166666666667</v>
       </c>
@@ -3514,7 +3512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3570,7 +3568,7 @@
       <c r="Q16" s="1">
         <v>1</v>
       </c>
-      <c r="R16" s="24">
+      <c r="R16" s="25">
         <f t="shared" si="5"/>
         <v>1524.4166666666667</v>
       </c>
@@ -3578,7 +3576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -3634,7 +3632,7 @@
       <c r="Q17" s="1">
         <v>1</v>
       </c>
-      <c r="R17" s="24">
+      <c r="R17" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3706,7 +3704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -3762,7 +3760,7 @@
       <c r="Q19" s="1">
         <v>1</v>
       </c>
-      <c r="R19" s="24">
+      <c r="R19" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3770,7 +3768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
@@ -3834,7 +3832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -3890,7 +3888,7 @@
       <c r="Q21" s="1">
         <v>1</v>
       </c>
-      <c r="R21" s="24">
+      <c r="R21" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -3898,7 +3896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -3954,7 +3952,7 @@
       <c r="Q22" s="1">
         <v>1</v>
       </c>
-      <c r="R22" s="24">
+      <c r="R22" s="25">
         <f t="shared" si="5"/>
         <v>1108.6666666666667</v>
       </c>
@@ -3962,7 +3960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -4018,7 +4016,7 @@
       <c r="Q23" s="1">
         <v>1</v>
       </c>
-      <c r="R23" s="24">
+      <c r="R23" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -4026,7 +4024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -4082,7 +4080,7 @@
       <c r="Q24" s="1">
         <v>1</v>
       </c>
-      <c r="R24" s="24">
+      <c r="R24" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -4090,7 +4088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -4146,7 +4144,7 @@
       <c r="Q25" s="1">
         <v>1</v>
       </c>
-      <c r="R25" s="24">
+      <c r="R25" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -4154,7 +4152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -4210,7 +4208,7 @@
       <c r="Q26" s="1">
         <v>1</v>
       </c>
-      <c r="R26" s="24">
+      <c r="R26" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -4218,7 +4216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -4274,7 +4272,7 @@
       <c r="Q27" s="1">
         <v>1</v>
       </c>
-      <c r="R27" s="24">
+      <c r="R27" s="25">
         <f t="shared" si="5"/>
         <v>3865.9</v>
       </c>
@@ -4282,7 +4280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -4338,7 +4336,7 @@
       <c r="Q28" s="1">
         <v>1</v>
       </c>
-      <c r="R28" s="24">
+      <c r="R28" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -4346,7 +4344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -4402,7 +4400,7 @@
       <c r="Q29" s="1">
         <v>1</v>
       </c>
-      <c r="R29" s="24">
+      <c r="R29" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -4410,7 +4408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -4466,7 +4464,7 @@
       <c r="Q30" s="1">
         <v>1</v>
       </c>
-      <c r="R30" s="24">
+      <c r="R30" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -4474,7 +4472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -4530,7 +4528,7 @@
       <c r="Q31" s="1">
         <v>1</v>
       </c>
-      <c r="R31" s="24">
+      <c r="R31" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -4538,7 +4536,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>133</v>
       </c>
@@ -4594,7 +4592,7 @@
       <c r="Q32" s="1">
         <v>1</v>
       </c>
-      <c r="R32" s="24">
+      <c r="R32" s="25">
         <f t="shared" si="5"/>
         <v>325.05</v>
       </c>
@@ -4602,7 +4600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -4654,7 +4652,7 @@
       <c r="Q33" s="1">
         <v>1</v>
       </c>
-      <c r="R33" s="24">
+      <c r="R33" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -4662,7 +4660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
@@ -4714,7 +4712,7 @@
       <c r="Q34" s="1">
         <v>1</v>
       </c>
-      <c r="R34" s="24">
+      <c r="R34" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -4722,7 +4720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
@@ -4774,7 +4772,7 @@
       <c r="Q35" s="1">
         <v>1</v>
       </c>
-      <c r="R35" s="24">
+      <c r="R35" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -4782,7 +4780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
@@ -4834,7 +4832,7 @@
       <c r="Q36" s="1">
         <v>1</v>
       </c>
-      <c r="R36" s="24">
+      <c r="R36" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -4842,7 +4840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
@@ -4894,7 +4892,7 @@
       <c r="Q37" s="1">
         <v>1</v>
       </c>
-      <c r="R37" s="24">
+      <c r="R37" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -4902,7 +4900,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -4954,7 +4952,7 @@
       <c r="Q38" s="1">
         <v>1</v>
       </c>
-      <c r="R38" s="24">
+      <c r="R38" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -4962,7 +4960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -5014,7 +5012,7 @@
       <c r="Q39" s="1">
         <v>1</v>
       </c>
-      <c r="R39" s="24">
+      <c r="R39" s="25">
         <f t="shared" si="5"/>
         <v>635</v>
       </c>
@@ -5022,7 +5020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -5074,7 +5072,7 @@
       <c r="Q40" s="1">
         <v>1</v>
       </c>
-      <c r="R40" s="24">
+      <c r="R40" s="25">
         <f t="shared" si="5"/>
         <v>582.08333333333326</v>
       </c>
@@ -5082,7 +5080,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -5138,7 +5136,7 @@
       <c r="Q41" s="1">
         <v>1</v>
       </c>
-      <c r="R41" s="24">
+      <c r="R41" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5210,7 +5208,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="17.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
@@ -5239,7 +5237,9 @@
       <c r="I43" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="K43" s="17">
         <v>45777</v>
       </c>
@@ -5254,19 +5254,25 @@
         <f>DATEDIF(E43,L43,"m")</f>
         <v>26</v>
       </c>
-      <c r="O43" s="23"/>
+      <c r="O43" s="21">
+        <v>1663</v>
+      </c>
       <c r="P43" s="21">
         <f>O43/12</f>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="24">
+        <v>138.58333333333334</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>1</v>
+      </c>
+      <c r="R43" s="25">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S43" s="1"/>
-    </row>
-    <row r="44" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+        <v>1663</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>12</v>
       </c>
@@ -5322,7 +5328,7 @@
       <c r="Q44" s="1">
         <v>1</v>
       </c>
-      <c r="R44" s="24">
+      <c r="R44" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -5330,7 +5336,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>12</v>
       </c>
@@ -5386,7 +5392,7 @@
       <c r="Q45" s="1">
         <v>1</v>
       </c>
-      <c r="R45" s="24">
+      <c r="R45" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5394,7 +5400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
@@ -5450,7 +5456,7 @@
       <c r="Q46" s="1">
         <v>1</v>
       </c>
-      <c r="R46" s="24">
+      <c r="R46" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5458,7 +5464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>12</v>
       </c>
@@ -5514,7 +5520,7 @@
       <c r="Q47" s="1">
         <v>1</v>
       </c>
-      <c r="R47" s="24">
+      <c r="R47" s="25">
         <f t="shared" si="5"/>
         <v>1247.25</v>
       </c>
@@ -5522,7 +5528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
@@ -5578,7 +5584,7 @@
       <c r="Q48" s="1">
         <v>1</v>
       </c>
-      <c r="R48" s="24">
+      <c r="R48" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5586,7 +5592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>12</v>
       </c>
@@ -5642,7 +5648,7 @@
       <c r="Q49" s="1">
         <v>1</v>
       </c>
-      <c r="R49" s="24">
+      <c r="R49" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5650,7 +5656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>12</v>
       </c>
@@ -5706,7 +5712,7 @@
       <c r="Q50" s="1">
         <v>1</v>
       </c>
-      <c r="R50" s="24">
+      <c r="R50" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5714,7 +5720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
@@ -5770,7 +5776,7 @@
       <c r="Q51" s="1">
         <v>1</v>
       </c>
-      <c r="R51" s="24">
+      <c r="R51" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -5778,7 +5784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
@@ -5834,7 +5840,7 @@
       <c r="Q52" s="1">
         <v>1</v>
       </c>
-      <c r="R52" s="24">
+      <c r="R52" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -5906,7 +5912,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -5962,7 +5968,7 @@
       <c r="Q54" s="1">
         <v>1</v>
       </c>
-      <c r="R54" s="24">
+      <c r="R54" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -5970,7 +5976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
@@ -6026,7 +6032,7 @@
       <c r="Q55" s="1">
         <v>1</v>
       </c>
-      <c r="R55" s="24">
+      <c r="R55" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -6034,7 +6040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>12</v>
       </c>
@@ -6090,7 +6096,7 @@
       <c r="Q56" s="1">
         <v>1</v>
       </c>
-      <c r="R56" s="24">
+      <c r="R56" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -6098,7 +6104,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -6154,7 +6160,7 @@
       <c r="Q57" s="1">
         <v>1</v>
       </c>
-      <c r="R57" s="24">
+      <c r="R57" s="25">
         <f t="shared" si="5"/>
         <v>1794.5</v>
       </c>
@@ -6162,7 +6168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>12</v>
       </c>
@@ -6218,7 +6224,7 @@
       <c r="Q58" s="1">
         <v>1</v>
       </c>
-      <c r="R58" s="24">
+      <c r="R58" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -6226,7 +6232,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>12</v>
       </c>
@@ -6282,7 +6288,7 @@
       <c r="Q59" s="1">
         <v>1</v>
       </c>
-      <c r="R59" s="24">
+      <c r="R59" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -6290,7 +6296,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>12</v>
       </c>
@@ -6346,7 +6352,7 @@
       <c r="Q60" s="1">
         <v>1</v>
       </c>
-      <c r="R60" s="24">
+      <c r="R60" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -6354,7 +6360,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>12</v>
       </c>
@@ -6410,7 +6416,7 @@
       <c r="Q61" s="1">
         <v>1</v>
       </c>
-      <c r="R61" s="24">
+      <c r="R61" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -6418,7 +6424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>12</v>
       </c>
@@ -6474,7 +6480,7 @@
       <c r="Q62" s="1">
         <v>1</v>
       </c>
-      <c r="R62" s="24">
+      <c r="R62" s="25">
         <f t="shared" si="5"/>
         <v>1663</v>
       </c>
@@ -6482,7 +6488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
@@ -6538,7 +6544,7 @@
       <c r="Q63" s="1">
         <v>1</v>
       </c>
-      <c r="R63" s="24">
+      <c r="R63" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -6546,7 +6552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>84</v>
       </c>
@@ -6610,7 +6616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>12</v>
       </c>
@@ -6666,7 +6672,7 @@
       <c r="Q65" s="1">
         <v>1</v>
       </c>
-      <c r="R65" s="24">
+      <c r="R65" s="25">
         <f t="shared" si="5"/>
         <v>1524.4166666666667</v>
       </c>
@@ -6674,7 +6680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>12</v>
       </c>
@@ -6730,7 +6736,7 @@
       <c r="Q66" s="1">
         <v>1</v>
       </c>
-      <c r="R66" s="24">
+      <c r="R66" s="25">
         <f t="shared" si="5"/>
         <v>298.8</v>
       </c>
@@ -6738,7 +6744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>84</v>
       </c>
@@ -6802,7 +6808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>12</v>
       </c>
@@ -6858,7 +6864,7 @@
       <c r="Q68" s="1">
         <v>1</v>
       </c>
-      <c r="R68" s="24">
+      <c r="R68" s="25">
         <f t="shared" ref="R68:R131" si="53">IF(N68&lt;=12,N68*P68,O68)</f>
         <v>1663</v>
       </c>
@@ -6866,7 +6872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>12</v>
       </c>
@@ -6922,7 +6928,7 @@
       <c r="Q69" s="1">
         <v>1</v>
       </c>
-      <c r="R69" s="24">
+      <c r="R69" s="25">
         <f t="shared" si="53"/>
         <v>1108.6666666666667</v>
       </c>
@@ -6930,7 +6936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
@@ -6986,7 +6992,7 @@
       <c r="Q70" s="1">
         <v>1</v>
       </c>
-      <c r="R70" s="24">
+      <c r="R70" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -6994,7 +7000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>12</v>
       </c>
@@ -7023,32 +7029,42 @@
       <c r="I71" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="J71" s="1"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
+      <c r="J71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K71" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L71" s="17">
+        <v>46142</v>
+      </c>
       <c r="M71" s="16">
         <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="N71" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N71" s="16">
         <f>DATEDIF(E71,L71,"m")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O71" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="O71" s="23">
+        <v>1498</v>
+      </c>
       <c r="P71" s="21">
         <f>O71/12</f>
-        <v>0</v>
-      </c>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>1</v>
+      </c>
+      <c r="R71" s="25">
         <f t="shared" si="53"/>
-        <v>#NUM!</v>
+        <v>1123.5</v>
       </c>
       <c r="S71" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -7104,7 +7120,7 @@
       <c r="Q72" s="1">
         <v>1</v>
       </c>
-      <c r="R72" s="24">
+      <c r="R72" s="25">
         <f t="shared" si="53"/>
         <v>1794.5</v>
       </c>
@@ -7112,7 +7128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>133</v>
       </c>
@@ -7168,7 +7184,7 @@
       <c r="Q73" s="1">
         <v>1</v>
       </c>
-      <c r="R73" s="24">
+      <c r="R73" s="25">
         <f t="shared" si="53"/>
         <v>325.05</v>
       </c>
@@ -7176,7 +7192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>12</v>
       </c>
@@ -7232,7 +7248,7 @@
       <c r="Q74" s="1">
         <v>1</v>
       </c>
-      <c r="R74" s="24">
+      <c r="R74" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7240,7 +7256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>84</v>
       </c>
@@ -7304,7 +7320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>12</v>
       </c>
@@ -7360,7 +7376,7 @@
       <c r="Q76" s="1">
         <v>1</v>
       </c>
-      <c r="R76" s="24">
+      <c r="R76" s="25">
         <f t="shared" si="53"/>
         <v>1385.8333333333335</v>
       </c>
@@ -7368,7 +7384,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>12</v>
       </c>
@@ -7424,7 +7440,7 @@
       <c r="Q77" s="1">
         <v>1</v>
       </c>
-      <c r="R77" s="24">
+      <c r="R77" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7432,7 +7448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>12</v>
       </c>
@@ -7488,7 +7504,7 @@
       <c r="Q78" s="1">
         <v>1</v>
       </c>
-      <c r="R78" s="24">
+      <c r="R78" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7496,7 +7512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>12</v>
       </c>
@@ -7552,7 +7568,7 @@
       <c r="Q79" s="1">
         <v>1</v>
       </c>
-      <c r="R79" s="24">
+      <c r="R79" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7560,7 +7576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>12</v>
       </c>
@@ -7616,7 +7632,7 @@
       <c r="Q80" s="1">
         <v>1</v>
       </c>
-      <c r="R80" s="24">
+      <c r="R80" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -7624,7 +7640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>12</v>
       </c>
@@ -7680,7 +7696,7 @@
       <c r="Q81" s="1">
         <v>1</v>
       </c>
-      <c r="R81" s="24">
+      <c r="R81" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -7688,7 +7704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>12</v>
       </c>
@@ -7744,7 +7760,7 @@
       <c r="Q82" s="1">
         <v>1</v>
       </c>
-      <c r="R82" s="24">
+      <c r="R82" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7752,7 +7768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>12</v>
       </c>
@@ -7808,7 +7824,7 @@
       <c r="Q83" s="1">
         <v>1</v>
       </c>
-      <c r="R83" s="24">
+      <c r="R83" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7816,7 +7832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>12</v>
       </c>
@@ -7872,7 +7888,7 @@
       <c r="Q84" s="1">
         <v>1</v>
       </c>
-      <c r="R84" s="24">
+      <c r="R84" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -7880,7 +7896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
@@ -7936,7 +7952,7 @@
       <c r="Q85" s="1">
         <v>1</v>
       </c>
-      <c r="R85" s="24">
+      <c r="R85" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -7944,7 +7960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -8000,7 +8016,7 @@
       <c r="Q86" s="1">
         <v>1</v>
       </c>
-      <c r="R86" s="24">
+      <c r="R86" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8008,7 +8024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -8064,7 +8080,7 @@
       <c r="Q87" s="1">
         <v>1</v>
       </c>
-      <c r="R87" s="24">
+      <c r="R87" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8072,7 +8088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
@@ -8136,7 +8152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
@@ -8192,7 +8208,7 @@
       <c r="Q89" s="1">
         <v>1</v>
       </c>
-      <c r="R89" s="24">
+      <c r="R89" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -8200,7 +8216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -8256,7 +8272,7 @@
       <c r="Q90" s="1">
         <v>1</v>
       </c>
-      <c r="R90" s="24">
+      <c r="R90" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -8264,7 +8280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -8320,7 +8336,7 @@
       <c r="Q91" s="1">
         <v>1</v>
       </c>
-      <c r="R91" s="24">
+      <c r="R91" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8328,7 +8344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>12</v>
       </c>
@@ -8384,7 +8400,7 @@
       <c r="Q92" s="1">
         <v>1</v>
       </c>
-      <c r="R92" s="24">
+      <c r="R92" s="25">
         <f t="shared" si="53"/>
         <v>970.08333333333337</v>
       </c>
@@ -8392,7 +8408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
@@ -8448,7 +8464,7 @@
       <c r="Q93" s="1">
         <v>1</v>
       </c>
-      <c r="R93" s="24">
+      <c r="R93" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8456,7 +8472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>84</v>
       </c>
@@ -8520,7 +8536,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
@@ -8576,7 +8592,7 @@
       <c r="Q95" s="1">
         <v>1</v>
       </c>
-      <c r="R95" s="24">
+      <c r="R95" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -8584,7 +8600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>12</v>
       </c>
@@ -8640,7 +8656,7 @@
       <c r="Q96" s="1">
         <v>1</v>
       </c>
-      <c r="R96" s="24">
+      <c r="R96" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8648,7 +8664,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>12</v>
       </c>
@@ -8704,7 +8720,7 @@
       <c r="Q97" s="1">
         <v>1</v>
       </c>
-      <c r="R97" s="24">
+      <c r="R97" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8712,7 +8728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>12</v>
       </c>
@@ -8768,7 +8784,7 @@
       <c r="Q98" s="1">
         <v>1</v>
       </c>
-      <c r="R98" s="24">
+      <c r="R98" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8776,7 +8792,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -8832,7 +8848,7 @@
       <c r="Q99" s="1">
         <v>1</v>
       </c>
-      <c r="R99" s="24">
+      <c r="R99" s="25">
         <f t="shared" si="53"/>
         <v>1794.5</v>
       </c>
@@ -8840,7 +8856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>12</v>
       </c>
@@ -8896,7 +8912,7 @@
       <c r="Q100" s="1">
         <v>1</v>
       </c>
-      <c r="R100" s="24">
+      <c r="R100" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -8904,7 +8920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>12</v>
       </c>
@@ -8960,7 +8976,7 @@
       <c r="Q101" s="1">
         <v>1</v>
       </c>
-      <c r="R101" s="24">
+      <c r="R101" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -8968,7 +8984,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>12</v>
       </c>
@@ -9024,7 +9040,7 @@
       <c r="Q102" s="1">
         <v>1</v>
       </c>
-      <c r="R102" s="24">
+      <c r="R102" s="25">
         <f t="shared" si="53"/>
         <v>1385.8333333333335</v>
       </c>
@@ -9096,7 +9112,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>12</v>
       </c>
@@ -9152,7 +9168,7 @@
       <c r="Q104" s="1">
         <v>1</v>
       </c>
-      <c r="R104" s="24">
+      <c r="R104" s="25">
         <f t="shared" si="53"/>
         <v>1108.6666666666667</v>
       </c>
@@ -9160,7 +9176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>12</v>
       </c>
@@ -9216,7 +9232,7 @@
       <c r="Q105" s="1">
         <v>1</v>
       </c>
-      <c r="R105" s="24">
+      <c r="R105" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -9224,7 +9240,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>12</v>
       </c>
@@ -9280,7 +9296,7 @@
       <c r="Q106" s="1">
         <v>1</v>
       </c>
-      <c r="R106" s="24">
+      <c r="R106" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -9288,7 +9304,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>12</v>
       </c>
@@ -9344,7 +9360,7 @@
       <c r="Q107" s="1">
         <v>1</v>
       </c>
-      <c r="R107" s="24">
+      <c r="R107" s="25">
         <f t="shared" si="53"/>
         <v>970.08333333333337</v>
       </c>
@@ -9352,7 +9368,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>12</v>
       </c>
@@ -9408,7 +9424,7 @@
       <c r="Q108" s="1">
         <v>1</v>
       </c>
-      <c r="R108" s="24">
+      <c r="R108" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -9416,7 +9432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>12</v>
       </c>
@@ -9445,32 +9461,42 @@
       <c r="I109" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J109" s="1"/>
-      <c r="K109" s="16"/>
-      <c r="L109" s="16"/>
+      <c r="J109" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K109" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L109" s="17">
+        <v>46142</v>
+      </c>
       <c r="M109" s="16">
         <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="N109" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N109" s="16">
         <f>DATEDIF(E109,L109,"m")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O109" s="23"/>
+        <v>7</v>
+      </c>
+      <c r="O109" s="23">
+        <v>1498</v>
+      </c>
       <c r="P109" s="21">
         <f>O109/12</f>
-        <v>0</v>
-      </c>
-      <c r="Q109" s="1"/>
-      <c r="R109" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q109" s="1">
+        <v>1</v>
+      </c>
+      <c r="R109" s="25">
         <f t="shared" si="53"/>
-        <v>#NUM!</v>
+        <v>873.83333333333326</v>
       </c>
       <c r="S109" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>12</v>
       </c>
@@ -9526,7 +9552,7 @@
       <c r="Q110" s="1">
         <v>1</v>
       </c>
-      <c r="R110" s="24">
+      <c r="R110" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -9534,7 +9560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
@@ -9590,7 +9616,7 @@
       <c r="Q111" s="1">
         <v>1</v>
       </c>
-      <c r="R111" s="24">
+      <c r="R111" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -9598,7 +9624,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>12</v>
       </c>
@@ -9654,7 +9680,7 @@
       <c r="Q112" s="1">
         <v>1</v>
       </c>
-      <c r="R112" s="24">
+      <c r="R112" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -9662,7 +9688,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>84</v>
       </c>
@@ -9726,7 +9752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>12</v>
       </c>
@@ -9782,7 +9808,7 @@
       <c r="Q114" s="1">
         <v>1</v>
       </c>
-      <c r="R114" s="24">
+      <c r="R114" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -9790,7 +9816,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>12</v>
       </c>
@@ -9846,7 +9872,7 @@
       <c r="Q115" s="1">
         <v>1</v>
       </c>
-      <c r="R115" s="24">
+      <c r="R115" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -9854,7 +9880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>12</v>
       </c>
@@ -9910,7 +9936,7 @@
       <c r="Q116" s="1">
         <v>1</v>
       </c>
-      <c r="R116" s="24">
+      <c r="R116" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -9918,7 +9944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
@@ -9974,7 +10000,7 @@
       <c r="Q117" s="1">
         <v>1</v>
       </c>
-      <c r="R117" s="24">
+      <c r="R117" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -9982,7 +10008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>84</v>
       </c>
@@ -10046,7 +10072,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>12</v>
       </c>
@@ -10102,7 +10128,7 @@
       <c r="Q119" s="1">
         <v>1</v>
       </c>
-      <c r="R119" s="24">
+      <c r="R119" s="25">
         <f t="shared" si="53"/>
         <v>1108.6666666666667</v>
       </c>
@@ -10110,7 +10136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>12</v>
       </c>
@@ -10166,7 +10192,7 @@
       <c r="Q120" s="1">
         <v>1</v>
       </c>
-      <c r="R120" s="24">
+      <c r="R120" s="25">
         <f t="shared" si="53"/>
         <v>1108.6666666666667</v>
       </c>
@@ -10174,7 +10200,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>12</v>
       </c>
@@ -10230,7 +10256,7 @@
       <c r="Q121" s="1">
         <v>1</v>
       </c>
-      <c r="R121" s="24">
+      <c r="R121" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -10238,7 +10264,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>12</v>
       </c>
@@ -10294,7 +10320,7 @@
       <c r="Q122" s="1">
         <v>1</v>
       </c>
-      <c r="R122" s="24">
+      <c r="R122" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -10302,7 +10328,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>12</v>
       </c>
@@ -10331,26 +10357,36 @@
       <c r="I123" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J123" s="1"/>
-      <c r="K123" s="16"/>
-      <c r="L123" s="16"/>
+      <c r="J123" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K123" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L123" s="17">
+        <v>46142</v>
+      </c>
       <c r="M123" s="16">
         <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="N123" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N123" s="16">
         <f t="shared" si="92"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O123" s="23"/>
+        <v>11</v>
+      </c>
+      <c r="O123" s="23">
+        <v>1498</v>
+      </c>
       <c r="P123" s="21">
         <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Q123" s="1"/>
-      <c r="R123" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>1</v>
+      </c>
+      <c r="R123" s="25">
         <f t="shared" si="53"/>
-        <v>#NUM!</v>
+        <v>1373.1666666666665</v>
       </c>
       <c r="S123" s="1" t="s">
         <v>19</v>
@@ -10484,7 +10520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>84</v>
       </c>
@@ -10540,7 +10576,7 @@
       <c r="Q126" s="1">
         <v>1</v>
       </c>
-      <c r="R126" s="26">
+      <c r="R126" s="25">
         <f t="shared" si="53"/>
         <v>1373.8999999999999</v>
       </c>
@@ -10548,7 +10584,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>84</v>
       </c>
@@ -10612,7 +10648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>12</v>
       </c>
@@ -10668,7 +10704,7 @@
       <c r="Q128" s="1">
         <v>1</v>
       </c>
-      <c r="R128" s="24">
+      <c r="R128" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -10676,7 +10712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>12</v>
       </c>
@@ -10732,7 +10768,7 @@
       <c r="Q129" s="1">
         <v>1</v>
       </c>
-      <c r="R129" s="24">
+      <c r="R129" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -10740,7 +10776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>12</v>
       </c>
@@ -10796,7 +10832,7 @@
       <c r="Q130" s="1">
         <v>1</v>
       </c>
-      <c r="R130" s="24">
+      <c r="R130" s="25">
         <f t="shared" si="53"/>
         <v>1663</v>
       </c>
@@ -10804,7 +10840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>12</v>
       </c>
@@ -10860,7 +10896,7 @@
       <c r="Q131" s="1">
         <v>1</v>
       </c>
-      <c r="R131" s="24">
+      <c r="R131" s="25">
         <f t="shared" si="53"/>
         <v>298.8</v>
       </c>
@@ -10868,7 +10904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>12</v>
       </c>
@@ -10924,7 +10960,7 @@
       <c r="Q132" s="1">
         <v>1</v>
       </c>
-      <c r="R132" s="24">
+      <c r="R132" s="25">
         <f t="shared" ref="R132:R192" si="99">IF(N132&lt;=12,N132*P132,O132)</f>
         <v>1663</v>
       </c>
@@ -10932,7 +10968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -10988,7 +11024,7 @@
       <c r="Q133" s="1">
         <v>1</v>
       </c>
-      <c r="R133" s="24">
+      <c r="R133" s="25">
         <f t="shared" si="99"/>
         <v>1794.5</v>
       </c>
@@ -10996,7 +11032,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>12</v>
       </c>
@@ -11052,7 +11088,7 @@
       <c r="Q134" s="1">
         <v>1</v>
       </c>
-      <c r="R134" s="24">
+      <c r="R134" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -11060,7 +11096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>12</v>
       </c>
@@ -11116,7 +11152,7 @@
       <c r="Q135" s="1">
         <v>1</v>
       </c>
-      <c r="R135" s="24">
+      <c r="R135" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -11124,7 +11160,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>12</v>
       </c>
@@ -11180,7 +11216,7 @@
       <c r="Q136" s="1">
         <v>1</v>
       </c>
-      <c r="R136" s="24">
+      <c r="R136" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -11188,7 +11224,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>12</v>
       </c>
@@ -11244,7 +11280,7 @@
       <c r="Q137" s="1">
         <v>1</v>
       </c>
-      <c r="R137" s="24">
+      <c r="R137" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11252,7 +11288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>12</v>
       </c>
@@ -11308,7 +11344,7 @@
       <c r="Q138" s="1">
         <v>1</v>
       </c>
-      <c r="R138" s="24">
+      <c r="R138" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11316,7 +11352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>12</v>
       </c>
@@ -11372,7 +11408,7 @@
       <c r="Q139" s="1">
         <v>1</v>
       </c>
-      <c r="R139" s="24">
+      <c r="R139" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11380,7 +11416,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
@@ -11436,7 +11472,7 @@
       <c r="Q140" s="1">
         <v>1</v>
       </c>
-      <c r="R140" s="24">
+      <c r="R140" s="25">
         <f t="shared" si="99"/>
         <v>236.4</v>
       </c>
@@ -11444,7 +11480,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>12</v>
       </c>
@@ -11500,7 +11536,7 @@
       <c r="Q141" s="1">
         <v>1</v>
       </c>
-      <c r="R141" s="24">
+      <c r="R141" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11572,7 +11608,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>12</v>
       </c>
@@ -11628,7 +11664,7 @@
       <c r="Q143" s="1">
         <v>1</v>
       </c>
-      <c r="R143" s="24">
+      <c r="R143" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11636,7 +11672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>12</v>
       </c>
@@ -11692,7 +11728,7 @@
       <c r="Q144" s="1">
         <v>1</v>
       </c>
-      <c r="R144" s="24">
+      <c r="R144" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11700,7 +11736,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>84</v>
       </c>
@@ -11764,7 +11800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>12</v>
       </c>
@@ -11820,7 +11856,7 @@
       <c r="Q146" s="1">
         <v>1</v>
       </c>
-      <c r="R146" s="24">
+      <c r="R146" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11828,7 +11864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>12</v>
       </c>
@@ -11884,7 +11920,7 @@
       <c r="Q147" s="1">
         <v>1</v>
       </c>
-      <c r="R147" s="24">
+      <c r="R147" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -11892,7 +11928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>12</v>
       </c>
@@ -11948,7 +11984,7 @@
       <c r="Q148" s="1">
         <v>1</v>
       </c>
-      <c r="R148" s="24">
+      <c r="R148" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -11956,7 +11992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>12</v>
       </c>
@@ -12012,7 +12048,7 @@
       <c r="Q149" s="1">
         <v>1</v>
       </c>
-      <c r="R149" s="24">
+      <c r="R149" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -12020,7 +12056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>12</v>
       </c>
@@ -12076,7 +12112,7 @@
       <c r="Q150" s="1">
         <v>1</v>
       </c>
-      <c r="R150" s="24">
+      <c r="R150" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -12148,7 +12184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>12</v>
       </c>
@@ -12204,7 +12240,7 @@
       <c r="Q152" s="1">
         <v>1</v>
       </c>
-      <c r="R152" s="24">
+      <c r="R152" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -12212,7 +12248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>133</v>
       </c>
@@ -12268,7 +12304,7 @@
       <c r="Q153" s="1">
         <v>1</v>
       </c>
-      <c r="R153" s="24">
+      <c r="R153" s="25">
         <f t="shared" si="99"/>
         <v>1373.8999999999999</v>
       </c>
@@ -12276,7 +12312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>12</v>
       </c>
@@ -12332,7 +12368,7 @@
       <c r="Q154" s="1">
         <v>1</v>
       </c>
-      <c r="R154" s="24">
+      <c r="R154" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -12340,7 +12376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>12</v>
       </c>
@@ -12396,7 +12432,7 @@
       <c r="Q155" s="1">
         <v>1</v>
       </c>
-      <c r="R155" s="24">
+      <c r="R155" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -12404,7 +12440,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>12</v>
       </c>
@@ -12460,7 +12496,7 @@
       <c r="Q156" s="1">
         <v>1</v>
       </c>
-      <c r="R156" s="24">
+      <c r="R156" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -12468,7 +12504,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>12</v>
       </c>
@@ -12524,7 +12560,7 @@
       <c r="Q157" s="1">
         <v>1</v>
       </c>
-      <c r="R157" s="24">
+      <c r="R157" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -12532,7 +12568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>12</v>
       </c>
@@ -12588,7 +12624,7 @@
       <c r="Q158" s="1">
         <v>1</v>
       </c>
-      <c r="R158" s="24">
+      <c r="R158" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -12596,7 +12632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>12</v>
       </c>
@@ -12625,32 +12661,42 @@
       <c r="I159" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J159" s="1"/>
-      <c r="K159" s="16"/>
-      <c r="L159" s="16"/>
+      <c r="J159" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K159" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L159" s="17">
+        <v>46142</v>
+      </c>
       <c r="M159" s="16">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="N159" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N159" s="16">
         <f t="shared" si="126"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O159" s="23"/>
+        <v>17</v>
+      </c>
+      <c r="O159" s="23">
+        <v>1498</v>
+      </c>
       <c r="P159" s="21">
         <f t="shared" si="127"/>
-        <v>0</v>
-      </c>
-      <c r="Q159" s="1"/>
-      <c r="R159" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>1</v>
+      </c>
+      <c r="R159" s="25">
         <f t="shared" si="99"/>
-        <v>#NUM!</v>
+        <v>1498</v>
       </c>
       <c r="S159" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>84</v>
       </c>
@@ -12714,7 +12760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>12</v>
       </c>
@@ -12770,7 +12816,7 @@
       <c r="Q161" s="1">
         <v>1</v>
       </c>
-      <c r="R161" s="24">
+      <c r="R161" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -12778,7 +12824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>12</v>
       </c>
@@ -12834,15 +12880,14 @@
       <c r="Q162" s="1">
         <v>1</v>
       </c>
-      <c r="R162" s="24" t="str">
-        <f t="shared" si="99"/>
-        <v>3.865,9</v>
+      <c r="R162" s="25">
+        <v>3865.9</v>
       </c>
       <c r="S162" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>5</v>
       </c>
@@ -12898,7 +12943,7 @@
       <c r="Q163" s="1">
         <v>1</v>
       </c>
-      <c r="R163" s="24">
+      <c r="R163" s="25">
         <f t="shared" si="99"/>
         <v>1794.5</v>
       </c>
@@ -12906,7 +12951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>12</v>
       </c>
@@ -12962,7 +13007,7 @@
       <c r="Q164" s="1">
         <v>1</v>
       </c>
-      <c r="R164" s="24">
+      <c r="R164" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -13098,7 +13143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>12</v>
       </c>
@@ -13154,7 +13199,7 @@
       <c r="Q167" s="1">
         <v>1</v>
       </c>
-      <c r="R167" s="24">
+      <c r="R167" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -13162,7 +13207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>12</v>
       </c>
@@ -13218,7 +13263,7 @@
       <c r="Q168" s="1">
         <v>1</v>
       </c>
-      <c r="R168" s="24">
+      <c r="R168" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -13226,7 +13271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>133</v>
       </c>
@@ -13282,7 +13327,7 @@
       <c r="Q169" s="1">
         <v>1</v>
       </c>
-      <c r="R169" s="24">
+      <c r="R169" s="25">
         <f t="shared" si="99"/>
         <v>325.05</v>
       </c>
@@ -13290,7 +13335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>133</v>
       </c>
@@ -13346,7 +13391,7 @@
       <c r="Q170" s="1">
         <v>1</v>
       </c>
-      <c r="R170" s="24">
+      <c r="R170" s="25">
         <f t="shared" si="99"/>
         <v>630.66666666666674</v>
       </c>
@@ -13354,7 +13399,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>12</v>
       </c>
@@ -13410,7 +13455,7 @@
       <c r="Q171" s="1">
         <v>1</v>
       </c>
-      <c r="R171" s="24">
+      <c r="R171" s="25">
         <f t="shared" si="99"/>
         <v>970.08333333333337</v>
       </c>
@@ -13418,7 +13463,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>84</v>
       </c>
@@ -13482,7 +13527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>12</v>
       </c>
@@ -13538,7 +13583,7 @@
       <c r="Q173" s="1">
         <v>1</v>
       </c>
-      <c r="R173" s="24">
+      <c r="R173" s="25">
         <f t="shared" si="99"/>
         <v>1385.8333333333335</v>
       </c>
@@ -13546,7 +13591,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
@@ -13602,7 +13647,7 @@
       <c r="Q174" s="1">
         <v>1</v>
       </c>
-      <c r="R174" s="24">
+      <c r="R174" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -13610,7 +13655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>12</v>
       </c>
@@ -13666,7 +13711,7 @@
       <c r="Q175" s="1">
         <v>1</v>
       </c>
-      <c r="R175" s="24">
+      <c r="R175" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -13674,7 +13719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>12</v>
       </c>
@@ -13703,26 +13748,36 @@
       <c r="I176" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J176" s="1"/>
-      <c r="K176" s="16"/>
-      <c r="L176" s="16"/>
+      <c r="J176" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K176" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L176" s="17">
+        <v>46142</v>
+      </c>
       <c r="M176" s="16">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="N176" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N176" s="16">
         <f t="shared" ref="N176:N180" si="143">DATEDIF(E176,L176,"m")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O176" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="O176" s="23">
+        <v>1498</v>
+      </c>
       <c r="P176" s="21">
         <f t="shared" ref="P176:P179" si="144">O176/12</f>
-        <v>0</v>
-      </c>
-      <c r="Q176" s="1"/>
-      <c r="R176" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q176" s="1">
+        <v>1</v>
+      </c>
+      <c r="R176" s="25">
         <f t="shared" si="99"/>
-        <v>#NUM!</v>
+        <v>1123.5</v>
       </c>
       <c r="S176" s="1" t="s">
         <v>19</v>
@@ -13792,7 +13847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>12</v>
       </c>
@@ -13848,7 +13903,7 @@
       <c r="Q178" s="1">
         <v>1</v>
       </c>
-      <c r="R178" s="24">
+      <c r="R178" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -13856,7 +13911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>12</v>
       </c>
@@ -13912,7 +13967,7 @@
       <c r="Q179" s="1">
         <v>1</v>
       </c>
-      <c r="R179" s="24">
+      <c r="R179" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -13920,7 +13975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>12</v>
       </c>
@@ -13976,7 +14031,7 @@
       <c r="Q180" s="1">
         <v>1</v>
       </c>
-      <c r="R180" s="24">
+      <c r="R180" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -13984,7 +14039,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>12</v>
       </c>
@@ -14013,26 +14068,36 @@
       <c r="I181" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J181" s="1"/>
-      <c r="K181" s="16"/>
-      <c r="L181" s="16"/>
+      <c r="J181" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K181" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L181" s="17">
+        <v>46142</v>
+      </c>
       <c r="M181" s="16">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="N181" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N181" s="16">
         <f>DATEDIF(E181,L181,"m")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O181" s="23"/>
+        <v>17</v>
+      </c>
+      <c r="O181" s="23">
+        <v>1498</v>
+      </c>
       <c r="P181" s="21">
         <f>O181/12</f>
-        <v>0</v>
-      </c>
-      <c r="Q181" s="1"/>
-      <c r="R181" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q181" s="1">
+        <v>1</v>
+      </c>
+      <c r="R181" s="25">
         <f t="shared" si="99"/>
-        <v>#NUM!</v>
+        <v>1498</v>
       </c>
       <c r="S181" s="1" t="s">
         <v>19</v>
@@ -14102,7 +14167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>12</v>
       </c>
@@ -14158,7 +14223,7 @@
       <c r="Q183" s="1">
         <v>1</v>
       </c>
-      <c r="R183" s="24">
+      <c r="R183" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14166,7 +14231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>12</v>
       </c>
@@ -14222,7 +14287,7 @@
       <c r="Q184" s="1">
         <v>1</v>
       </c>
-      <c r="R184" s="24">
+      <c r="R184" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14230,7 +14295,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>12</v>
       </c>
@@ -14286,7 +14351,7 @@
       <c r="Q185" s="1">
         <v>1</v>
       </c>
-      <c r="R185" s="24">
+      <c r="R185" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14294,7 +14359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>12</v>
       </c>
@@ -14323,32 +14388,42 @@
       <c r="I186" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J186" s="1"/>
-      <c r="K186" s="16"/>
-      <c r="L186" s="16"/>
+      <c r="J186" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K186" s="17">
+        <v>45777</v>
+      </c>
+      <c r="L186" s="17">
+        <v>46142</v>
+      </c>
       <c r="M186" s="16">
         <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
-      <c r="N186" s="16" t="e">
+        <v>12</v>
+      </c>
+      <c r="N186" s="16">
         <f t="shared" si="147"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O186" s="23"/>
+        <v>10</v>
+      </c>
+      <c r="O186" s="23">
+        <v>1498</v>
+      </c>
       <c r="P186" s="21">
         <f t="shared" si="148"/>
-        <v>0</v>
-      </c>
-      <c r="Q186" s="1"/>
-      <c r="R186" s="24" t="e">
+        <v>124.83333333333333</v>
+      </c>
+      <c r="Q186" s="1">
+        <v>1</v>
+      </c>
+      <c r="R186" s="25">
         <f t="shared" si="99"/>
-        <v>#NUM!</v>
+        <v>1248.3333333333333</v>
       </c>
       <c r="S186" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>12</v>
       </c>
@@ -14404,7 +14479,7 @@
       <c r="Q187" s="1">
         <v>1</v>
       </c>
-      <c r="R187" s="24">
+      <c r="R187" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14412,7 +14487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>12</v>
       </c>
@@ -14468,7 +14543,7 @@
       <c r="Q188" s="1">
         <v>1</v>
       </c>
-      <c r="R188" s="24">
+      <c r="R188" s="25">
         <f t="shared" si="99"/>
         <v>298.8</v>
       </c>
@@ -14476,7 +14551,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>12</v>
       </c>
@@ -14532,7 +14607,7 @@
       <c r="Q189" s="1">
         <v>1</v>
       </c>
-      <c r="R189" s="24">
+      <c r="R189" s="25">
         <f t="shared" si="99"/>
         <v>1108.6666666666667</v>
       </c>
@@ -14540,7 +14615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>12</v>
       </c>
@@ -14596,7 +14671,7 @@
       <c r="Q190" s="1">
         <v>1</v>
       </c>
-      <c r="R190" s="24">
+      <c r="R190" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14604,7 +14679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>12</v>
       </c>
@@ -14660,7 +14735,7 @@
       <c r="Q191" s="1">
         <v>1</v>
       </c>
-      <c r="R191" s="24">
+      <c r="R191" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14668,7 +14743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>12</v>
       </c>
@@ -14724,7 +14799,7 @@
       <c r="Q192" s="1">
         <v>1</v>
       </c>
-      <c r="R192" s="24">
+      <c r="R192" s="25">
         <f t="shared" si="99"/>
         <v>1663</v>
       </c>
@@ -14744,19 +14819,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S192" xr:uid="{F403300F-DC30-4742-B09D-03B69867D524}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="FLEXIVEL-JGS"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Exchange Online (Plan 2)"/>
-        <filter val="Intune"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S192" xr:uid="{F403300F-DC30-4742-B09D-03B69867D524}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>